<commit_message>
all JSON directory files updated
</commit_message>
<xml_diff>
--- a/JSON/Roles.xlsx
+++ b/JSON/Roles.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="110">
   <si>
     <t>Role</t>
   </si>
@@ -416,6 +416,18 @@
   </si>
   <si>
     <t>Vampires</t>
+  </si>
+  <si>
+    <t>Cursed</t>
+  </si>
+  <si>
+    <t>Village (until dead, then werewolf)</t>
+  </si>
+  <si>
+    <t>Old Man</t>
+  </si>
+  <si>
+    <t>Dies on night (# of Wolves) + 1</t>
   </si>
 </sst>
 </file>
@@ -797,15 +809,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" style="3"/>
+    <col min="2" max="2" width="17.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="49" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="5"/>
@@ -1404,22 +1416,50 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="6">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>